<commit_message>
adding dept date arrival times
</commit_message>
<xml_diff>
--- a/mvc/downloads/paxfeed.xlsx
+++ b/mvc/downloads/paxfeed.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21805"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="219" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{4EE21D03-9A9F-4154-84BA-75D2BF9ED567}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B33790E0-0B3B-4A3B-80D2-D8AF8B49B294}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="80">
   <si>
     <t>Airline Code</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>dept date</t>
+  </si>
+  <si>
+    <t>arrival date</t>
+  </si>
+  <si>
+    <t>dept time</t>
+  </si>
+  <si>
+    <t>arrival time</t>
   </si>
   <si>
     <t>class</t>
@@ -298,10 +307,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -617,20 +627,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T30"/>
+  <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3:N30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.5703125" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -691,25 +702,34 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G2">
         <v>1233456789</v>
@@ -718,60 +738,69 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K2" s="2">
         <v>43614</v>
       </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="L2" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O2" t="s">
         <v>29</v>
       </c>
-      <c r="P2">
-        <v>9989910254</v>
+      <c r="P2" t="s">
+        <v>30</v>
       </c>
       <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2">
+        <v>9989910254</v>
       </c>
       <c r="T2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G3">
         <v>1233456789</v>
@@ -780,60 +809,69 @@
         <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2">
         <v>43614</v>
       </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P3">
-        <v>9989910254</v>
+      <c r="L3" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3">
+        <v>9989910254</v>
       </c>
       <c r="T3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>1233456789</v>
@@ -842,60 +880,69 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K4" s="2">
         <v>43614</v>
       </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4">
-        <v>9989910254</v>
+      <c r="L4" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O4" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" t="s">
+        <v>30</v>
       </c>
       <c r="Q4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R4" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4">
+        <v>9989910254</v>
       </c>
       <c r="T4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U4" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G5">
         <v>1233456789</v>
@@ -904,60 +951,69 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2">
         <v>43614</v>
       </c>
-      <c r="L5" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="1" t="s">
+      <c r="L5" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O5" t="s">
         <v>29</v>
       </c>
-      <c r="P5">
-        <v>9989910254</v>
+      <c r="P5" t="s">
+        <v>30</v>
       </c>
       <c r="Q5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5">
+        <v>9989910254</v>
       </c>
       <c r="T5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
+      <c r="W5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G6">
         <v>1233456789</v>
@@ -966,60 +1022,69 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2">
         <v>43614</v>
       </c>
-      <c r="L6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6">
-        <v>9989910254</v>
+      <c r="L6" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P6" t="s">
+        <v>30</v>
       </c>
       <c r="Q6" t="s">
-        <v>30</v>
-      </c>
-      <c r="R6" t="s">
-        <v>39</v>
-      </c>
-      <c r="S6" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6">
+        <v>9989910254</v>
       </c>
       <c r="T6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U6" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G7">
         <v>1233456789</v>
@@ -1028,60 +1093,69 @@
         <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K7" s="2">
         <v>43614</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O7" t="s">
+        <v>45</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7">
+        <v>9989910254</v>
+      </c>
+      <c r="T7" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" t="s">
         <v>42</v>
       </c>
-      <c r="M7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N7" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7">
-        <v>9989910254</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>30</v>
-      </c>
-      <c r="R7" t="s">
-        <v>39</v>
-      </c>
-      <c r="S7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="V7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <v>1233456789</v>
@@ -1090,60 +1164,69 @@
         <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K8" s="2">
         <v>43614</v>
       </c>
-      <c r="L8" t="s">
-        <v>45</v>
-      </c>
-      <c r="M8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8">
-        <v>9989910254</v>
+      <c r="L8" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" t="s">
+        <v>30</v>
       </c>
       <c r="Q8" t="s">
-        <v>30</v>
-      </c>
-      <c r="R8" t="s">
-        <v>39</v>
-      </c>
-      <c r="S8" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S8">
+        <v>9989910254</v>
       </c>
       <c r="T8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U8" t="s">
+        <v>42</v>
+      </c>
+      <c r="V8" t="s">
+        <v>34</v>
+      </c>
+      <c r="W8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>1233456789</v>
@@ -1152,60 +1235,69 @@
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K9" s="2">
         <v>43614</v>
       </c>
-      <c r="L9" t="s">
-        <v>48</v>
-      </c>
-      <c r="M9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N9" t="s">
-        <v>28</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9">
-        <v>9989910254</v>
+      <c r="L9" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
       </c>
       <c r="Q9" t="s">
-        <v>30</v>
-      </c>
-      <c r="R9" t="s">
-        <v>39</v>
-      </c>
-      <c r="S9" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9">
+        <v>9989910254</v>
       </c>
       <c r="T9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U9" t="s">
+        <v>42</v>
+      </c>
+      <c r="V9" t="s">
+        <v>34</v>
+      </c>
+      <c r="W9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>1233456789</v>
@@ -1214,60 +1306,69 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K10" s="2">
         <v>43614</v>
       </c>
-      <c r="L10" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" t="s">
-        <v>27</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10">
-        <v>9989910254</v>
+      <c r="L10" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O10" t="s">
+        <v>51</v>
+      </c>
+      <c r="P10" t="s">
+        <v>30</v>
       </c>
       <c r="Q10" t="s">
-        <v>30</v>
-      </c>
-      <c r="R10" t="s">
-        <v>39</v>
-      </c>
-      <c r="S10" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10">
+        <v>9989910254</v>
       </c>
       <c r="T10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U10" t="s">
+        <v>42</v>
+      </c>
+      <c r="V10" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G11">
         <v>1233456789</v>
@@ -1276,60 +1377,69 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K11" s="2">
         <v>43614</v>
       </c>
-      <c r="L11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N11" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11">
-        <v>9989910254</v>
+      <c r="L11" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O11" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" t="s">
+        <v>30</v>
       </c>
       <c r="Q11" t="s">
-        <v>30</v>
-      </c>
-      <c r="R11" t="s">
-        <v>52</v>
-      </c>
-      <c r="S11" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11">
+        <v>9989910254</v>
       </c>
       <c r="T11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U11" t="s">
+        <v>55</v>
+      </c>
+      <c r="V11" t="s">
+        <v>34</v>
+      </c>
+      <c r="W11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G12">
         <v>1233456789</v>
@@ -1338,60 +1448,69 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K12" s="2">
         <v>43614</v>
       </c>
-      <c r="L12" t="s">
-        <v>45</v>
-      </c>
-      <c r="M12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N12" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12">
-        <v>9989910254</v>
+      <c r="L12" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O12" t="s">
+        <v>48</v>
+      </c>
+      <c r="P12" t="s">
+        <v>30</v>
       </c>
       <c r="Q12" t="s">
-        <v>30</v>
-      </c>
-      <c r="R12" t="s">
-        <v>52</v>
-      </c>
-      <c r="S12" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S12">
+        <v>9989910254</v>
       </c>
       <c r="T12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U12" t="s">
+        <v>55</v>
+      </c>
+      <c r="V12" t="s">
+        <v>34</v>
+      </c>
+      <c r="W12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G13">
         <v>1233456789</v>
@@ -1400,60 +1519,69 @@
         <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K13" s="2">
         <v>43614</v>
       </c>
-      <c r="L13" t="s">
-        <v>48</v>
-      </c>
-      <c r="M13" t="s">
-        <v>27</v>
-      </c>
-      <c r="N13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P13">
-        <v>9989910254</v>
+      <c r="L13" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O13" t="s">
+        <v>51</v>
+      </c>
+      <c r="P13" t="s">
+        <v>30</v>
       </c>
       <c r="Q13" t="s">
-        <v>30</v>
-      </c>
-      <c r="R13" t="s">
-        <v>52</v>
-      </c>
-      <c r="S13" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13">
+        <v>9989910254</v>
       </c>
       <c r="T13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U13" t="s">
+        <v>55</v>
+      </c>
+      <c r="V13" t="s">
+        <v>34</v>
+      </c>
+      <c r="W13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G14">
         <v>1233456789</v>
@@ -1462,60 +1590,69 @@
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K14" s="2">
         <v>43614</v>
       </c>
-      <c r="L14" t="s">
-        <v>48</v>
-      </c>
-      <c r="M14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" t="s">
-        <v>28</v>
-      </c>
-      <c r="O14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P14">
-        <v>9989910254</v>
+      <c r="L14" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P14" t="s">
+        <v>30</v>
       </c>
       <c r="Q14" t="s">
-        <v>30</v>
-      </c>
-      <c r="R14" t="s">
-        <v>52</v>
-      </c>
-      <c r="S14" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14">
+        <v>9989910254</v>
       </c>
       <c r="T14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U14" t="s">
+        <v>55</v>
+      </c>
+      <c r="V14" t="s">
+        <v>34</v>
+      </c>
+      <c r="W14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G15">
         <v>1233456789</v>
@@ -1524,60 +1661,69 @@
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J15" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K15" s="2">
         <v>43614</v>
       </c>
-      <c r="L15" t="s">
-        <v>42</v>
-      </c>
-      <c r="M15" t="s">
-        <v>27</v>
-      </c>
-      <c r="N15" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15">
-        <v>9989910254</v>
+      <c r="L15" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O15" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" t="s">
+        <v>30</v>
       </c>
       <c r="Q15" t="s">
-        <v>30</v>
-      </c>
-      <c r="R15" t="s">
-        <v>52</v>
-      </c>
-      <c r="S15" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15">
+        <v>9989910254</v>
       </c>
       <c r="T15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U15" t="s">
+        <v>55</v>
+      </c>
+      <c r="V15" t="s">
+        <v>34</v>
+      </c>
+      <c r="W15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G16">
         <v>1233456789</v>
@@ -1586,60 +1732,69 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K16" s="2">
         <v>43614</v>
       </c>
-      <c r="L16" t="s">
-        <v>45</v>
-      </c>
-      <c r="M16" t="s">
-        <v>27</v>
-      </c>
-      <c r="N16" t="s">
-        <v>28</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P16">
-        <v>9989910254</v>
+      <c r="L16" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O16" t="s">
+        <v>48</v>
+      </c>
+      <c r="P16" t="s">
+        <v>30</v>
       </c>
       <c r="Q16" t="s">
-        <v>30</v>
-      </c>
-      <c r="R16" t="s">
-        <v>27</v>
-      </c>
-      <c r="S16" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S16">
+        <v>9989910254</v>
       </c>
       <c r="T16" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U16" t="s">
+        <v>30</v>
+      </c>
+      <c r="V16" t="s">
+        <v>34</v>
+      </c>
+      <c r="W16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G17">
         <v>1233456789</v>
@@ -1648,60 +1803,69 @@
         <v>22</v>
       </c>
       <c r="I17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J17" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K17" s="2">
         <v>43614</v>
       </c>
-      <c r="L17" t="s">
-        <v>48</v>
-      </c>
-      <c r="M17" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" t="s">
-        <v>28</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17">
-        <v>9989910254</v>
+      <c r="L17" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O17" t="s">
+        <v>51</v>
+      </c>
+      <c r="P17" t="s">
+        <v>30</v>
       </c>
       <c r="Q17" t="s">
-        <v>30</v>
-      </c>
-      <c r="R17" t="s">
-        <v>27</v>
-      </c>
-      <c r="S17" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17">
+        <v>9989910254</v>
       </c>
       <c r="T17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U17" t="s">
+        <v>30</v>
+      </c>
+      <c r="V17" t="s">
+        <v>34</v>
+      </c>
+      <c r="W17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G18">
         <v>1233456789</v>
@@ -1710,60 +1874,69 @@
         <v>11</v>
       </c>
       <c r="I18" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J18" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K18" s="2">
         <v>43614</v>
       </c>
-      <c r="L18" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" t="s">
-        <v>27</v>
-      </c>
-      <c r="N18" t="s">
-        <v>28</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P18">
-        <v>9989910254</v>
+      <c r="L18" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O18" t="s">
+        <v>45</v>
+      </c>
+      <c r="P18" t="s">
+        <v>30</v>
       </c>
       <c r="Q18" t="s">
-        <v>30</v>
-      </c>
-      <c r="R18" t="s">
-        <v>27</v>
-      </c>
-      <c r="S18" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18">
+        <v>9989910254</v>
       </c>
       <c r="T18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U18" t="s">
+        <v>30</v>
+      </c>
+      <c r="V18" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G19">
         <v>1233456789</v>
@@ -1772,60 +1945,69 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J19" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K19" s="2">
         <v>43614</v>
       </c>
-      <c r="L19" t="s">
-        <v>45</v>
-      </c>
-      <c r="M19" t="s">
-        <v>27</v>
-      </c>
-      <c r="N19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P19">
-        <v>9989910254</v>
+      <c r="L19" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N19" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O19" t="s">
+        <v>48</v>
+      </c>
+      <c r="P19" t="s">
+        <v>30</v>
       </c>
       <c r="Q19" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" t="s">
-        <v>27</v>
-      </c>
-      <c r="S19" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19">
+        <v>9989910254</v>
       </c>
       <c r="T19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V19" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G20">
         <v>1233456789</v>
@@ -1834,60 +2016,69 @@
         <v>11</v>
       </c>
       <c r="I20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J20" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K20" s="2">
         <v>43614</v>
       </c>
-      <c r="L20" t="s">
-        <v>48</v>
-      </c>
-      <c r="M20" t="s">
-        <v>27</v>
-      </c>
-      <c r="N20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P20">
-        <v>9989910254</v>
+      <c r="L20" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N20" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" t="s">
+        <v>30</v>
       </c>
       <c r="Q20" t="s">
-        <v>30</v>
-      </c>
-      <c r="R20" t="s">
-        <v>27</v>
-      </c>
-      <c r="S20" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S20">
+        <v>9989910254</v>
       </c>
       <c r="T20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G21">
         <v>1233456789</v>
@@ -1896,60 +2087,69 @@
         <v>22</v>
       </c>
       <c r="I21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J21" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K21" s="2">
         <v>43614</v>
       </c>
-      <c r="L21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M21" t="s">
-        <v>27</v>
-      </c>
-      <c r="N21" t="s">
-        <v>28</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21">
-        <v>9989910254</v>
+      <c r="L21" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N21" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O21" t="s">
+        <v>45</v>
+      </c>
+      <c r="P21" t="s">
+        <v>30</v>
       </c>
       <c r="Q21" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" t="s">
-        <v>27</v>
-      </c>
-      <c r="S21" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S21">
+        <v>9989910254</v>
       </c>
       <c r="T21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U21" t="s">
+        <v>30</v>
+      </c>
+      <c r="V21" t="s">
+        <v>34</v>
+      </c>
+      <c r="W21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F22" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G22">
         <v>1233456789</v>
@@ -1958,60 +2158,69 @@
         <v>22</v>
       </c>
       <c r="I22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K22" s="2">
         <v>43614</v>
       </c>
-      <c r="L22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M22" t="s">
-        <v>27</v>
-      </c>
-      <c r="N22" t="s">
-        <v>28</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22">
-        <v>9989910254</v>
+      <c r="L22" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M22" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N22" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O22" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" t="s">
+        <v>30</v>
       </c>
       <c r="Q22" t="s">
-        <v>30</v>
-      </c>
-      <c r="R22" t="s">
-        <v>27</v>
-      </c>
-      <c r="S22" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S22">
+        <v>9989910254</v>
       </c>
       <c r="T22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U22" t="s">
+        <v>30</v>
+      </c>
+      <c r="V22" t="s">
+        <v>34</v>
+      </c>
+      <c r="W22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E23" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G23">
         <v>1233456789</v>
@@ -2020,60 +2229,69 @@
         <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J23" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K23" s="2">
         <v>43614</v>
       </c>
-      <c r="L23" t="s">
-        <v>48</v>
-      </c>
-      <c r="M23" t="s">
-        <v>27</v>
-      </c>
-      <c r="N23" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23">
-        <v>9989910254</v>
+      <c r="L23" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N23" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O23" t="s">
+        <v>51</v>
+      </c>
+      <c r="P23" t="s">
+        <v>30</v>
       </c>
       <c r="Q23" t="s">
-        <v>30</v>
-      </c>
-      <c r="R23" t="s">
-        <v>27</v>
-      </c>
-      <c r="S23" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S23">
+        <v>9989910254</v>
       </c>
       <c r="T23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V23" t="s">
+        <v>34</v>
+      </c>
+      <c r="W23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G24">
         <v>1233456789</v>
@@ -2082,60 +2300,69 @@
         <v>22</v>
       </c>
       <c r="I24" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J24" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K24" s="2">
         <v>43614</v>
       </c>
-      <c r="L24" t="s">
-        <v>42</v>
-      </c>
-      <c r="M24" t="s">
-        <v>27</v>
-      </c>
-      <c r="N24" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24">
-        <v>9989910254</v>
+      <c r="L24" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M24" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N24" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O24" t="s">
+        <v>45</v>
+      </c>
+      <c r="P24" t="s">
+        <v>30</v>
       </c>
       <c r="Q24" t="s">
-        <v>30</v>
-      </c>
-      <c r="R24" t="s">
-        <v>27</v>
-      </c>
-      <c r="S24" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S24">
+        <v>9989910254</v>
       </c>
       <c r="T24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U24" t="s">
+        <v>30</v>
+      </c>
+      <c r="V24" t="s">
+        <v>34</v>
+      </c>
+      <c r="W24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F25" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G25">
         <v>1233456789</v>
@@ -2144,60 +2371,69 @@
         <v>22</v>
       </c>
       <c r="I25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K25" s="2">
         <v>43614</v>
       </c>
-      <c r="L25" t="s">
-        <v>70</v>
-      </c>
-      <c r="M25" t="s">
-        <v>27</v>
-      </c>
-      <c r="N25" t="s">
-        <v>28</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25">
-        <v>9989910254</v>
+      <c r="L25" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O25" t="s">
+        <v>73</v>
+      </c>
+      <c r="P25" t="s">
+        <v>30</v>
       </c>
       <c r="Q25" t="s">
-        <v>30</v>
-      </c>
-      <c r="R25" t="s">
-        <v>27</v>
-      </c>
-      <c r="S25" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S25">
+        <v>9989910254</v>
       </c>
       <c r="T25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U25" t="s">
+        <v>30</v>
+      </c>
+      <c r="V25" t="s">
+        <v>34</v>
+      </c>
+      <c r="W25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G26">
         <v>1233456789</v>
@@ -2206,60 +2442,69 @@
         <v>22</v>
       </c>
       <c r="I26" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K26" s="2">
         <v>43614</v>
       </c>
-      <c r="L26" t="s">
-        <v>72</v>
-      </c>
-      <c r="M26" t="s">
-        <v>27</v>
-      </c>
-      <c r="N26" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26">
-        <v>9989910254</v>
+      <c r="L26" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N26" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O26" t="s">
+        <v>75</v>
+      </c>
+      <c r="P26" t="s">
+        <v>30</v>
       </c>
       <c r="Q26" t="s">
-        <v>30</v>
-      </c>
-      <c r="R26" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S26">
+        <v>9989910254</v>
       </c>
       <c r="T26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U26" t="s">
+        <v>30</v>
+      </c>
+      <c r="V26" t="s">
+        <v>34</v>
+      </c>
+      <c r="W26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C27">
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G27">
         <v>1233456789</v>
@@ -2268,60 +2513,69 @@
         <v>22</v>
       </c>
       <c r="I27" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J27" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K27" s="2">
         <v>43614</v>
       </c>
-      <c r="L27" t="s">
-        <v>74</v>
-      </c>
-      <c r="M27" t="s">
-        <v>27</v>
-      </c>
-      <c r="N27" t="s">
-        <v>28</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27">
-        <v>9989910254</v>
+      <c r="L27" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N27" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O27" t="s">
+        <v>77</v>
+      </c>
+      <c r="P27" t="s">
+        <v>30</v>
       </c>
       <c r="Q27" t="s">
-        <v>30</v>
-      </c>
-      <c r="R27" t="s">
-        <v>27</v>
-      </c>
-      <c r="S27" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S27">
+        <v>9989910254</v>
       </c>
       <c r="T27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U27" t="s">
+        <v>30</v>
+      </c>
+      <c r="V27" t="s">
+        <v>34</v>
+      </c>
+      <c r="W27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G28">
         <v>1233456789</v>
@@ -2330,60 +2584,69 @@
         <v>22</v>
       </c>
       <c r="I28" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K28" s="2">
         <v>43614</v>
       </c>
-      <c r="L28" t="s">
-        <v>75</v>
-      </c>
-      <c r="M28" t="s">
-        <v>27</v>
-      </c>
-      <c r="N28" t="s">
-        <v>28</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P28">
-        <v>9989910254</v>
+      <c r="L28" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O28" t="s">
+        <v>78</v>
+      </c>
+      <c r="P28" t="s">
+        <v>30</v>
       </c>
       <c r="Q28" t="s">
-        <v>30</v>
-      </c>
-      <c r="R28" t="s">
-        <v>27</v>
-      </c>
-      <c r="S28" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S28">
+        <v>9989910254</v>
       </c>
       <c r="T28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U28" t="s">
+        <v>30</v>
+      </c>
+      <c r="V28" t="s">
+        <v>34</v>
+      </c>
+      <c r="W28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C29">
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F29" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G29">
         <v>1233456789</v>
@@ -2392,60 +2655,69 @@
         <v>22</v>
       </c>
       <c r="I29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K29" s="2">
         <v>43614</v>
       </c>
-      <c r="L29" t="s">
-        <v>70</v>
-      </c>
-      <c r="M29" t="s">
-        <v>27</v>
-      </c>
-      <c r="N29" t="s">
-        <v>28</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29">
-        <v>9989910254</v>
+      <c r="L29" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O29" t="s">
+        <v>73</v>
+      </c>
+      <c r="P29" t="s">
+        <v>30</v>
       </c>
       <c r="Q29" t="s">
-        <v>30</v>
-      </c>
-      <c r="R29" t="s">
-        <v>27</v>
-      </c>
-      <c r="S29" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S29">
+        <v>9989910254</v>
       </c>
       <c r="T29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
+        <v>33</v>
+      </c>
+      <c r="U29" t="s">
+        <v>30</v>
+      </c>
+      <c r="V29" t="s">
+        <v>34</v>
+      </c>
+      <c r="W29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C30">
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F30" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G30">
         <v>1233456789</v>
@@ -2454,58 +2726,67 @@
         <v>22</v>
       </c>
       <c r="I30" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="J30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K30" s="2">
         <v>43614</v>
       </c>
-      <c r="L30" t="s">
-        <v>72</v>
-      </c>
-      <c r="M30" t="s">
-        <v>27</v>
-      </c>
-      <c r="N30" t="s">
-        <v>28</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P30">
-        <v>9989910254</v>
+      <c r="L30" s="2">
+        <v>43615</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="N30" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="O30" t="s">
+        <v>75</v>
+      </c>
+      <c r="P30" t="s">
+        <v>30</v>
       </c>
       <c r="Q30" t="s">
-        <v>30</v>
-      </c>
-      <c r="R30" t="s">
-        <v>27</v>
-      </c>
-      <c r="S30" t="s">
-        <v>31</v>
+        <v>31</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="S30">
+        <v>9989910254</v>
       </c>
       <c r="T30" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="U30" t="s">
+        <v>30</v>
+      </c>
+      <c r="V30" t="s">
+        <v>34</v>
+      </c>
+      <c r="W30" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{6D2DA717-9711-4511-B83C-515B4F6EEC2E}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{8648E4D3-46C5-44E9-8240-D44C04C1ACF1}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{4FE92DAF-2852-4B12-BB7B-17E0F6A0E43C}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{C86F9549-1235-41EB-8FE6-C1B536943206}"/>
-    <hyperlink ref="O6" r:id="rId5" xr:uid="{B0EFEE03-6199-4248-96DA-FADA9DF5FCC2}"/>
-    <hyperlink ref="O7" r:id="rId6" xr:uid="{E386B778-4987-46C2-9D40-02D016610E26}"/>
-    <hyperlink ref="O8" r:id="rId7" xr:uid="{4F0C40C6-FFCC-4524-B2C8-5E1BF8ED60A2}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{85577CBC-ADBC-4F21-9FBB-140320919391}"/>
-    <hyperlink ref="O10" r:id="rId9" xr:uid="{E4C165DD-4634-4771-9DE1-73C250E03134}"/>
-    <hyperlink ref="O11" r:id="rId10" xr:uid="{79CFF0A7-7249-47D8-B9B3-CDACBC539CA6}"/>
-    <hyperlink ref="O12" r:id="rId11" xr:uid="{43F05E98-8105-44EA-B97A-38DAF0C18EFC}"/>
-    <hyperlink ref="O13" r:id="rId12" xr:uid="{456108AB-B6AB-4117-ABAE-C4284558A1F9}"/>
-    <hyperlink ref="O14" r:id="rId13" xr:uid="{956B24DE-62A7-4E16-9401-3900661E036F}"/>
-    <hyperlink ref="O15" r:id="rId14" xr:uid="{DAC6C086-17EE-47B2-A9B5-CE3C3EE56D5A}"/>
+    <hyperlink ref="R2" r:id="rId1" xr:uid="{6D2DA717-9711-4511-B83C-515B4F6EEC2E}"/>
+    <hyperlink ref="R3" r:id="rId2" xr:uid="{8648E4D3-46C5-44E9-8240-D44C04C1ACF1}"/>
+    <hyperlink ref="R4" r:id="rId3" xr:uid="{4FE92DAF-2852-4B12-BB7B-17E0F6A0E43C}"/>
+    <hyperlink ref="R5" r:id="rId4" xr:uid="{C86F9549-1235-41EB-8FE6-C1B536943206}"/>
+    <hyperlink ref="R6" r:id="rId5" xr:uid="{B0EFEE03-6199-4248-96DA-FADA9DF5FCC2}"/>
+    <hyperlink ref="R7" r:id="rId6" xr:uid="{E386B778-4987-46C2-9D40-02D016610E26}"/>
+    <hyperlink ref="R8" r:id="rId7" xr:uid="{4F0C40C6-FFCC-4524-B2C8-5E1BF8ED60A2}"/>
+    <hyperlink ref="R9" r:id="rId8" xr:uid="{85577CBC-ADBC-4F21-9FBB-140320919391}"/>
+    <hyperlink ref="R10" r:id="rId9" xr:uid="{E4C165DD-4634-4771-9DE1-73C250E03134}"/>
+    <hyperlink ref="R11" r:id="rId10" xr:uid="{79CFF0A7-7249-47D8-B9B3-CDACBC539CA6}"/>
+    <hyperlink ref="R12" r:id="rId11" xr:uid="{43F05E98-8105-44EA-B97A-38DAF0C18EFC}"/>
+    <hyperlink ref="R13" r:id="rId12" xr:uid="{456108AB-B6AB-4117-ABAE-C4284558A1F9}"/>
+    <hyperlink ref="R14" r:id="rId13" xr:uid="{956B24DE-62A7-4E16-9401-3900661E036F}"/>
+    <hyperlink ref="R15" r:id="rId14" xr:uid="{DAC6C086-17EE-47B2-A9B5-CE3C3EE56D5A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding new format for pax
</commit_message>
<xml_diff>
--- a/mvc/downloads/paxfeed.xlsx
+++ b/mvc/downloads/paxfeed.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21916"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{887D49B6-5647-4FDE-AEA8-513FC8682F60}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{279593AC-6792-4933-9729-5C139A7F94A6}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="53">
   <si>
     <t>Airline Code</t>
   </si>
@@ -97,19 +97,19 @@
     <t>channel</t>
   </si>
   <si>
+    <t>WQ1235</t>
+  </si>
+  <si>
+    <t>Salini</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>ADT</t>
+  </si>
+  <si>
     <t>VX</t>
-  </si>
-  <si>
-    <t>WQ1235</t>
-  </si>
-  <si>
-    <t>Salini</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>ADT</t>
   </si>
   <si>
     <t>VX1234</t>
@@ -188,10 +188,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -214,15 +222,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,13 +546,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X16"/>
+  <dimension ref="A1:X30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" t="s">
@@ -618,23 +634,23 @@
       </c>
     </row>
     <row r="2" spans="1:24">
-      <c r="A2" t="s">
+      <c r="A2">
+        <v>618</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" t="s">
-        <v>28</v>
       </c>
       <c r="G2">
         <v>1233456789</v>
@@ -643,24 +659,24 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="2">
         <v>43614</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="2">
         <v>43615</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>1</v>
       </c>
       <c r="P2" t="s">
@@ -692,11 +708,11 @@
       </c>
     </row>
     <row r="3" spans="1:24">
-      <c r="A3" t="s">
+      <c r="A3">
+        <v>618</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -705,10 +721,10 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" t="s">
-        <v>28</v>
       </c>
       <c r="G3">
         <v>1233456789</v>
@@ -717,24 +733,24 @@
         <v>11</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="2">
         <v>43614</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="2">
         <v>43615</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N3" s="2">
+      <c r="N3" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>1</v>
       </c>
       <c r="P3" t="s">
@@ -766,11 +782,11 @@
       </c>
     </row>
     <row r="4" spans="1:24">
-      <c r="A4" t="s">
+      <c r="A4">
+        <v>618</v>
+      </c>
+      <c r="B4" t="s">
         <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -779,10 +795,10 @@
         <v>40</v>
       </c>
       <c r="E4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
       <c r="G4">
         <v>1233456789</v>
@@ -791,24 +807,24 @@
         <v>11</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
         <v>29</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="2">
         <v>43614</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="2">
         <v>43615</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
         <v>2</v>
       </c>
       <c r="P4" t="s">
@@ -840,11 +856,11 @@
       </c>
     </row>
     <row r="5" spans="1:24">
-      <c r="A5" t="s">
+      <c r="A5">
+        <v>618</v>
+      </c>
+      <c r="B5" t="s">
         <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>25</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -853,10 +869,10 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
       <c r="G5">
         <v>1233456789</v>
@@ -865,24 +881,24 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J5" t="s">
         <v>29</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>43614</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="2">
         <v>43615</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>3</v>
       </c>
       <c r="P5" t="s">
@@ -914,11 +930,11 @@
       </c>
     </row>
     <row r="6" spans="1:24">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>618</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -927,10 +943,10 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
       </c>
       <c r="G6">
         <v>1233456789</v>
@@ -939,24 +955,24 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J6" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="2">
         <v>43614</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="2">
         <v>43615</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>3</v>
       </c>
       <c r="P6" t="s">
@@ -988,23 +1004,23 @@
       </c>
     </row>
     <row r="7" spans="1:24">
-      <c r="A7" t="s">
+      <c r="A7">
+        <v>618</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
       </c>
       <c r="G7">
         <v>1233456789</v>
@@ -1013,24 +1029,24 @@
         <v>22</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="2">
         <v>43614</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="2">
         <v>43615</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
         <v>2</v>
       </c>
       <c r="P7" t="s">
@@ -1062,11 +1078,11 @@
       </c>
     </row>
     <row r="8" spans="1:24">
-      <c r="A8" t="s">
+      <c r="A8">
+        <v>618</v>
+      </c>
+      <c r="B8" t="s">
         <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1078,7 +1094,7 @@
         <v>47</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <v>1233456789</v>
@@ -1087,24 +1103,24 @@
         <v>22</v>
       </c>
       <c r="I8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J8" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="2">
         <v>43614</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="2">
         <v>43615</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <v>4</v>
       </c>
       <c r="P8" t="s">
@@ -1136,11 +1152,11 @@
       </c>
     </row>
     <row r="9" spans="1:24">
-      <c r="A9" t="s">
+      <c r="A9">
+        <v>618</v>
+      </c>
+      <c r="B9" t="s">
         <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1152,7 +1168,7 @@
         <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9">
         <v>1233456789</v>
@@ -1161,24 +1177,24 @@
         <v>22</v>
       </c>
       <c r="I9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J9" t="s">
         <v>45</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="2">
         <v>43614</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>43615</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
         <v>1</v>
       </c>
       <c r="P9" t="s">
@@ -1210,11 +1226,11 @@
       </c>
     </row>
     <row r="10" spans="1:24">
-      <c r="A10" t="s">
+      <c r="A10">
+        <v>618</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -1226,7 +1242,7 @@
         <v>49</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G10">
         <v>1233456789</v>
@@ -1235,24 +1251,24 @@
         <v>11</v>
       </c>
       <c r="I10" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J10" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="2">
         <v>43614</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="2">
         <v>43615</v>
       </c>
-      <c r="M10" s="2">
+      <c r="M10" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N10" s="2">
+      <c r="N10" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <v>1</v>
       </c>
       <c r="P10" t="s">
@@ -1284,11 +1300,11 @@
       </c>
     </row>
     <row r="11" spans="1:24">
-      <c r="A11" t="s">
+      <c r="A11">
+        <v>618</v>
+      </c>
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1300,7 +1316,7 @@
         <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G11">
         <v>1233456789</v>
@@ -1309,24 +1325,24 @@
         <v>11</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J11" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <v>43614</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>43615</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M11" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <v>2</v>
       </c>
       <c r="P11" t="s">
@@ -1358,23 +1374,23 @@
       </c>
     </row>
     <row r="12" spans="1:24">
-      <c r="A12" t="s">
+      <c r="A12">
+        <v>618</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>27</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
       </c>
       <c r="G12">
         <v>1233456789</v>
@@ -1383,24 +1399,24 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J12" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>43614</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="2">
         <v>43615</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M12" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <v>3</v>
       </c>
       <c r="P12" t="s">
@@ -1432,11 +1448,11 @@
       </c>
     </row>
     <row r="13" spans="1:24">
-      <c r="A13" t="s">
+      <c r="A13">
+        <v>618</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1445,10 +1461,10 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" t="s">
         <v>27</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
       </c>
       <c r="G13">
         <v>1233456789</v>
@@ -1457,24 +1473,24 @@
         <v>22</v>
       </c>
       <c r="I13" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J13" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="2">
         <v>43614</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="2">
         <v>43615</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <v>3</v>
       </c>
       <c r="P13" t="s">
@@ -1506,11 +1522,11 @@
       </c>
     </row>
     <row r="14" spans="1:24">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>618</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
       </c>
       <c r="C14">
         <v>3</v>
@@ -1519,10 +1535,10 @@
         <v>40</v>
       </c>
       <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" t="s">
         <v>27</v>
-      </c>
-      <c r="F14" t="s">
-        <v>28</v>
       </c>
       <c r="G14">
         <v>1233456789</v>
@@ -1531,24 +1547,24 @@
         <v>22</v>
       </c>
       <c r="I14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J14" t="s">
         <v>51</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <v>43614</v>
       </c>
-      <c r="L14" s="1">
+      <c r="L14" s="2">
         <v>43615</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <v>2</v>
       </c>
       <c r="P14" t="s">
@@ -1580,11 +1596,11 @@
       </c>
     </row>
     <row r="15" spans="1:24">
-      <c r="A15" t="s">
+      <c r="A15">
+        <v>618</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1593,10 +1609,10 @@
         <v>42</v>
       </c>
       <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" t="s">
         <v>27</v>
-      </c>
-      <c r="F15" t="s">
-        <v>28</v>
       </c>
       <c r="G15">
         <v>1233456789</v>
@@ -1605,24 +1621,24 @@
         <v>22</v>
       </c>
       <c r="I15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J15" t="s">
         <v>51</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="2">
         <v>43614</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="2">
         <v>43615</v>
       </c>
-      <c r="M15" s="2">
+      <c r="M15" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N15" s="2">
+      <c r="N15" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <v>4</v>
       </c>
       <c r="P15" t="s">
@@ -1654,11 +1670,11 @@
       </c>
     </row>
     <row r="16" spans="1:24">
-      <c r="A16" t="s">
+      <c r="A16">
+        <v>618</v>
+      </c>
+      <c r="B16" t="s">
         <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
       </c>
       <c r="C16">
         <v>5</v>
@@ -1667,10 +1683,10 @@
         <v>43</v>
       </c>
       <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
       </c>
       <c r="G16">
         <v>1233456789</v>
@@ -1679,24 +1695,24 @@
         <v>22</v>
       </c>
       <c r="I16" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J16" t="s">
         <v>51</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <v>43614</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="2">
         <v>43615</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="3">
         <v>0.4375</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="3">
         <v>0.6875</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="1">
         <v>4</v>
       </c>
       <c r="P16" t="s">
@@ -1726,6 +1742,61 @@
       <c r="X16" t="s">
         <v>37</v>
       </c>
+    </row>
+    <row r="17" spans="11:15">
+      <c r="K17" s="2"/>
+      <c r="O17" s="1"/>
+    </row>
+    <row r="18" spans="11:15">
+      <c r="K18" s="2"/>
+      <c r="O18" s="1"/>
+    </row>
+    <row r="19" spans="11:15">
+      <c r="K19" s="2"/>
+      <c r="O19" s="1"/>
+    </row>
+    <row r="20" spans="11:15">
+      <c r="K20" s="2"/>
+      <c r="O20" s="1"/>
+    </row>
+    <row r="21" spans="11:15">
+      <c r="K21" s="2"/>
+      <c r="O21" s="1"/>
+    </row>
+    <row r="22" spans="11:15">
+      <c r="K22" s="2"/>
+      <c r="O22" s="1"/>
+    </row>
+    <row r="23" spans="11:15">
+      <c r="K23" s="2"/>
+      <c r="O23" s="1"/>
+    </row>
+    <row r="24" spans="11:15">
+      <c r="K24" s="2"/>
+      <c r="O24" s="1"/>
+    </row>
+    <row r="25" spans="11:15">
+      <c r="K25" s="2"/>
+      <c r="O25" s="1"/>
+    </row>
+    <row r="26" spans="11:15">
+      <c r="K26" s="2"/>
+      <c r="O26" s="1"/>
+    </row>
+    <row r="27" spans="11:15">
+      <c r="K27" s="2"/>
+      <c r="O27" s="1"/>
+    </row>
+    <row r="28" spans="11:15">
+      <c r="K28" s="2"/>
+      <c r="O28" s="1"/>
+    </row>
+    <row r="29" spans="11:15">
+      <c r="K29" s="2"/>
+      <c r="O29" s="1"/>
+    </row>
+    <row r="30" spans="11:15">
+      <c r="O30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>